<commit_message>
Update to include new NERR stations
</commit_message>
<xml_diff>
--- a/data/StormTrackVariables.xlsx
+++ b/data/StormTrackVariables.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\RNERRS2\SWMPr_Storm_Story_Template-main\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BallengerJ\Documents\GitHub\SWMPr_Storm_Story_Template\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4DCF40F-BD10-4B2A-BF9E-0662FAEE6A64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="3"/>
+    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Multi-storm parameters" sheetId="1" r:id="rId1"/>
@@ -105,7 +106,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -135,17 +136,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{C9C70C01-3B6B-4A03-8D80-D26422EDDDA7}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -453,21 +454,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" customWidth="1"/>
-    <col min="2" max="2" width="69.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.54296875" customWidth="1"/>
+    <col min="2" max="2" width="69.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -478,7 +479,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -486,7 +487,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -497,12 +498,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -513,7 +514,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -524,7 +525,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -541,25 +542,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A2" sqref="A2:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.88671875" customWidth="1"/>
-    <col min="2" max="2" width="9.77734375" customWidth="1"/>
-    <col min="3" max="3" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="169.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="114" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="173.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -573,29 +574,27 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D6" t="s">
         <v>14</v>
       </c>
@@ -606,21 +605,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" customWidth="1"/>
-    <col min="2" max="2" width="69.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.54296875" customWidth="1"/>
+    <col min="2" max="2" width="69.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -631,7 +630,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -639,7 +638,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -650,12 +649,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -666,7 +665,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -677,7 +676,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -694,25 +693,25 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.44140625" customWidth="1"/>
-    <col min="2" max="2" width="9.77734375" customWidth="1"/>
-    <col min="3" max="3" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="175.5546875" customWidth="1"/>
+    <col min="1" max="1" width="33.453125" customWidth="1"/>
+    <col min="2" max="2" width="9.81640625" customWidth="1"/>
+    <col min="3" max="3" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="175.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -726,12 +725,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
-      <c r="B2" s="2"/>
-      <c r="C2">
-        <v>1</v>
-      </c>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D2" t="s">
         <v>14</v>
       </c>

</xml_diff>